<commit_message>
Archivo con datos actualizados
</commit_message>
<xml_diff>
--- a/Base de datos/Data in Excel/Resultados.xlsx
+++ b/Base de datos/Data in Excel/Resultados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documentos\Trabajos\Base de datos\Inventario_UG\Base de datos\Data in Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fire_\Documents\Trabajos\Base de datos\Inventario_UG\Base de datos\Data in Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3580510-9FF0-485E-9445-5197755DD7D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752EE6A5-85D8-4859-84D8-D2A01A7CDEAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9961C840-150E-47BC-9A7E-A77A29674DEC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9961C840-150E-47BC-9A7E-A77A29674DEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1559" uniqueCount="228">
   <si>
     <t>MXL7351V3J</t>
   </si>
@@ -711,6 +711,12 @@
   </si>
   <si>
     <t xml:space="preserve">Modelo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsable </t>
+  </si>
+  <si>
+    <t>Geovani Hernández Gómez</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC24D04A-B82F-47BE-9902-02A22BFFAACA}">
-  <dimension ref="A1:H227"/>
+  <dimension ref="A1:I227"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1095,7 @@
     <col min="8" max="8" width="17.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>219</v>
       </c>
@@ -1111,8 +1117,11 @@
       <c r="H1" s="3" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1137,8 +1146,11 @@
       <c r="H2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1163,8 +1175,11 @@
       <c r="H3" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1189,8 +1204,11 @@
       <c r="H4" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1215,8 +1233,11 @@
       <c r="H5" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1241,8 +1262,11 @@
       <c r="H6" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1267,8 +1291,11 @@
       <c r="H7" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1287,8 +1314,11 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1313,8 +1343,11 @@
       <c r="H9" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1339,8 +1372,11 @@
       <c r="H10" s="4">
         <v>4018</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1365,8 +1401,11 @@
       <c r="H11" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1391,8 +1430,11 @@
       <c r="H12" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1415,8 +1457,11 @@
       <c r="H13" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1441,8 +1486,11 @@
       <c r="H14" s="4" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1467,8 +1515,11 @@
       <c r="H15" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1493,8 +1544,11 @@
       <c r="H16" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1519,8 +1573,11 @@
       <c r="H17" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1545,8 +1602,11 @@
       <c r="H18" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1571,8 +1631,11 @@
       <c r="H19" s="4" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1597,8 +1660,11 @@
       <c r="H20" s="4">
         <v>900430020</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1623,8 +1689,11 @@
       <c r="H21" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1649,8 +1718,11 @@
       <c r="H22" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1675,8 +1747,11 @@
       <c r="H23" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1701,8 +1776,11 @@
       <c r="H24" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1727,8 +1805,11 @@
       <c r="H25" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1753,8 +1834,11 @@
       <c r="H26" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1779,8 +1863,11 @@
       <c r="H27" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1805,8 +1892,11 @@
       <c r="H28" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1831,8 +1921,11 @@
       <c r="H29" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1857,8 +1950,11 @@
       <c r="H30" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1883,8 +1979,11 @@
       <c r="H31" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1909,8 +2008,11 @@
       <c r="H32" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1935,8 +2037,11 @@
       <c r="H33" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1961,8 +2066,11 @@
       <c r="H34" s="4" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1987,8 +2095,11 @@
       <c r="H35" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -2013,8 +2124,11 @@
       <c r="H36" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -2039,8 +2153,11 @@
       <c r="H37" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2065,8 +2182,11 @@
       <c r="H38" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2091,8 +2211,11 @@
       <c r="H39" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2117,8 +2240,11 @@
       <c r="H40" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2143,8 +2269,11 @@
       <c r="H41" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2169,8 +2298,11 @@
       <c r="H42" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2195,8 +2327,11 @@
       <c r="H43" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2221,8 +2356,11 @@
       <c r="H44" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2247,8 +2385,11 @@
       <c r="H45" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2273,8 +2414,11 @@
       <c r="H46" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2299,8 +2443,11 @@
       <c r="H47" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -2325,8 +2472,11 @@
       <c r="H48" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2351,8 +2501,11 @@
       <c r="H49" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2377,8 +2530,11 @@
       <c r="H50" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2403,8 +2559,11 @@
       <c r="H51" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2429,8 +2588,11 @@
       <c r="H52" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2455,8 +2617,11 @@
       <c r="H53" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2481,8 +2646,11 @@
       <c r="H54" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2507,8 +2675,11 @@
       <c r="H55" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2533,8 +2704,11 @@
       <c r="H56" s="4" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2559,8 +2733,11 @@
       <c r="H57" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2585,8 +2762,11 @@
       <c r="H58" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2611,8 +2791,11 @@
       <c r="H59" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2637,8 +2820,11 @@
       <c r="H60" s="4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2663,8 +2849,11 @@
       <c r="H61" s="4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -2689,8 +2878,11 @@
       <c r="H62" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -2715,8 +2907,11 @@
       <c r="H63" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -2741,8 +2936,11 @@
       <c r="H64" s="4" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -2767,8 +2965,11 @@
       <c r="H65" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -2793,8 +2994,11 @@
       <c r="H66" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -2819,8 +3023,11 @@
       <c r="H67" s="4" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -2845,8 +3052,11 @@
       <c r="H68" s="4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -2871,8 +3081,11 @@
       <c r="H69" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -2897,8 +3110,11 @@
       <c r="H70" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -2923,8 +3139,11 @@
       <c r="H71" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -2949,8 +3168,11 @@
       <c r="H72" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -2975,8 +3197,11 @@
       <c r="H73" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -3001,8 +3226,11 @@
       <c r="H74" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -3027,8 +3255,11 @@
       <c r="H75" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -3053,8 +3284,11 @@
       <c r="H76" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -3079,8 +3313,11 @@
       <c r="H77" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -3105,8 +3342,11 @@
       <c r="H78" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -3131,8 +3371,11 @@
       <c r="H79" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -3157,8 +3400,11 @@
       <c r="H80" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -3183,8 +3429,11 @@
       <c r="H81" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -3209,8 +3458,11 @@
       <c r="H82" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -3235,8 +3487,11 @@
       <c r="H83" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -3261,8 +3516,11 @@
       <c r="H84" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -3287,8 +3545,11 @@
       <c r="H85" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -3313,8 +3574,11 @@
       <c r="H86" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -3339,8 +3603,11 @@
       <c r="H87" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -3365,8 +3632,11 @@
       <c r="H88" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -3391,8 +3661,11 @@
       <c r="H89" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -3417,8 +3690,11 @@
       <c r="H90" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -3443,8 +3719,11 @@
       <c r="H91" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -3469,8 +3748,11 @@
       <c r="H92" s="4" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -3495,8 +3777,11 @@
       <c r="H93" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -3521,8 +3806,11 @@
       <c r="H94" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -3547,8 +3835,11 @@
       <c r="H95" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -3573,8 +3864,11 @@
       <c r="H96" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -3599,8 +3893,11 @@
       <c r="H97" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -3625,8 +3922,11 @@
       <c r="H98" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -3651,8 +3951,11 @@
       <c r="H99" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -3677,8 +3980,11 @@
       <c r="H100" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -3703,8 +4009,11 @@
       <c r="H101" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -3729,8 +4038,11 @@
       <c r="H102" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -3755,8 +4067,11 @@
       <c r="H103" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -3781,8 +4096,11 @@
       <c r="H104" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -3807,8 +4125,11 @@
       <c r="H105" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -3833,8 +4154,11 @@
       <c r="H106" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -3859,8 +4183,11 @@
       <c r="H107" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -3885,8 +4212,11 @@
       <c r="H108" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -3911,8 +4241,11 @@
       <c r="H109" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -3937,8 +4270,11 @@
       <c r="H110" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -3963,8 +4299,11 @@
       <c r="H111" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -3989,8 +4328,11 @@
       <c r="H112" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -4015,8 +4357,11 @@
       <c r="H113" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -4041,8 +4386,11 @@
       <c r="H114" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I114" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -4067,8 +4415,11 @@
       <c r="H115" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -4093,8 +4444,11 @@
       <c r="H116" s="4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -4119,8 +4473,11 @@
       <c r="H117" s="4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -4145,8 +4502,11 @@
       <c r="H118" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -4171,8 +4531,11 @@
       <c r="H119" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -4197,8 +4560,11 @@
       <c r="H120" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -4223,8 +4589,11 @@
       <c r="H121" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -4249,8 +4618,11 @@
       <c r="H122" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -4275,8 +4647,11 @@
       <c r="H123" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I123" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -4301,8 +4676,11 @@
       <c r="H124" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -4327,8 +4705,11 @@
       <c r="H125" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -4353,8 +4734,11 @@
       <c r="H126" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I126" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -4379,8 +4763,11 @@
       <c r="H127" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -4405,8 +4792,11 @@
       <c r="H128" s="4" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -4431,8 +4821,11 @@
       <c r="H129" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I129" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -4457,8 +4850,11 @@
       <c r="H130" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I130" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -4483,8 +4879,11 @@
       <c r="H131" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I131" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -4509,8 +4908,11 @@
       <c r="H132" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -4535,8 +4937,11 @@
       <c r="H133" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I133" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -4561,8 +4966,11 @@
       <c r="H134" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I134" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -4587,8 +4995,11 @@
       <c r="H135" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I135" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -4613,8 +5024,11 @@
       <c r="H136" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I136" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -4639,8 +5053,11 @@
       <c r="H137" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I137" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -4665,8 +5082,11 @@
       <c r="H138" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I138" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -4691,8 +5111,11 @@
       <c r="H139" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I139" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -4717,8 +5140,11 @@
       <c r="H140" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I140" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -4743,8 +5169,11 @@
       <c r="H141" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I141" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -4769,8 +5198,11 @@
       <c r="H142" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I142" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -4795,8 +5227,11 @@
       <c r="H143" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I143" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -4821,8 +5256,11 @@
       <c r="H144" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I144" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -4847,8 +5285,11 @@
       <c r="H145" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I145" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -4873,8 +5314,11 @@
       <c r="H146" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I146" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -4899,8 +5343,11 @@
       <c r="H147" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I147" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -4925,8 +5372,11 @@
       <c r="H148" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I148" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -4951,8 +5401,11 @@
       <c r="H149" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I149" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -4977,8 +5430,11 @@
       <c r="H150" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I150" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -5003,8 +5459,11 @@
       <c r="H151" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I151" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -5029,8 +5488,11 @@
       <c r="H152" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I152" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -5055,8 +5517,11 @@
       <c r="H153" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I153" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -5081,8 +5546,11 @@
       <c r="H154" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I154" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -5107,8 +5575,11 @@
       <c r="H155" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I155" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -5133,8 +5604,11 @@
       <c r="H156" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I156" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -5159,8 +5633,11 @@
       <c r="H157" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I157" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -5185,8 +5662,11 @@
       <c r="H158" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I158" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -5211,8 +5691,11 @@
       <c r="H159" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I159" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -5237,8 +5720,11 @@
       <c r="H160" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I160" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -5263,8 +5749,11 @@
       <c r="H161" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I161" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -5289,8 +5778,11 @@
       <c r="H162" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I162" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -5315,8 +5807,11 @@
       <c r="H163" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I163" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -5341,8 +5836,11 @@
       <c r="H164" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I164" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -5367,8 +5865,11 @@
       <c r="H165" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I165" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -5393,8 +5894,11 @@
       <c r="H166" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I166" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -5419,8 +5923,11 @@
       <c r="H167" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I167" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -5445,8 +5952,11 @@
       <c r="H168" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I168" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -5471,8 +5981,11 @@
       <c r="H169" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I169" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -5497,8 +6010,11 @@
       <c r="H170" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I170" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -5523,8 +6039,11 @@
       <c r="H171" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I171" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -5549,8 +6068,11 @@
       <c r="H172" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I172" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -5575,8 +6097,11 @@
       <c r="H173" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I173" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -5601,8 +6126,11 @@
       <c r="H174" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I174" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -5627,8 +6155,11 @@
       <c r="H175" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I175" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -5653,8 +6184,11 @@
       <c r="H176" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I176" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -5679,8 +6213,11 @@
       <c r="H177" s="4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I177" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -5705,8 +6242,11 @@
       <c r="H178" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I178" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -5731,8 +6271,11 @@
       <c r="H179" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I179" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -5757,8 +6300,11 @@
       <c r="H180" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I180" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -5783,8 +6329,11 @@
       <c r="H181" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I181" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -5809,8 +6358,11 @@
       <c r="H182" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I182" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -5835,8 +6387,11 @@
       <c r="H183" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I183" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -5861,8 +6416,11 @@
       <c r="H184" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I184" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -5887,8 +6445,11 @@
       <c r="H185" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I185" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -5913,8 +6474,11 @@
       <c r="H186" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I186" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -5939,8 +6503,11 @@
       <c r="H187" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I187" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -5965,8 +6532,11 @@
       <c r="H188" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I188" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -5991,8 +6561,11 @@
       <c r="H189" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I189" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -6017,8 +6590,11 @@
       <c r="H190" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I190" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -6043,8 +6619,11 @@
       <c r="H191" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I191" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -6069,8 +6648,11 @@
       <c r="H192" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I192" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -6095,8 +6677,11 @@
       <c r="H193" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I193" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -6121,8 +6706,11 @@
       <c r="H194" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I194" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -6147,8 +6735,11 @@
       <c r="H195" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I195" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -6173,8 +6764,11 @@
       <c r="H196" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I196" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -6199,8 +6793,11 @@
       <c r="H197" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I197" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -6225,8 +6822,11 @@
       <c r="H198" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I198" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -6251,8 +6851,11 @@
       <c r="H199" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I199" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -6277,8 +6880,11 @@
       <c r="H200" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I200" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -6303,8 +6909,11 @@
       <c r="H201" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I201" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -6329,8 +6938,11 @@
       <c r="H202" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I202" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -6355,8 +6967,11 @@
       <c r="H203" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I203" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -6381,8 +6996,11 @@
       <c r="H204" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I204" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -6407,8 +7025,11 @@
       <c r="H205" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I205" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -6433,8 +7054,11 @@
       <c r="H206" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I206" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -6459,8 +7083,11 @@
       <c r="H207" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I207" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -6485,8 +7112,11 @@
       <c r="H208" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I208" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -6511,8 +7141,11 @@
       <c r="H209" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I209" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -6537,8 +7170,11 @@
       <c r="H210" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I210" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -6563,8 +7199,11 @@
       <c r="H211" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I211" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -6589,8 +7228,11 @@
       <c r="H212" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I212" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -6615,8 +7257,11 @@
       <c r="H213" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I213" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -6641,8 +7286,11 @@
       <c r="H214" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I214" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -6667,8 +7315,11 @@
       <c r="H215" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I215" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -6693,8 +7344,11 @@
       <c r="H216" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I216" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -6719,8 +7373,11 @@
       <c r="H217" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I217" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -6745,8 +7402,11 @@
       <c r="H218" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I218" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -6771,8 +7431,11 @@
       <c r="H219" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I219" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -6797,8 +7460,11 @@
       <c r="H220" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I220" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -6823,8 +7489,11 @@
       <c r="H221" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I221" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -6849,8 +7518,11 @@
       <c r="H222" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I222" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -6875,8 +7547,11 @@
       <c r="H223" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I223" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -6901,8 +7576,11 @@
       <c r="H224" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I224" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -6927,8 +7605,11 @@
       <c r="H225" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I225" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -6953,8 +7634,11 @@
       <c r="H226" s="4" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I226" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -6978,6 +7662,9 @@
       </c>
       <c r="H227" s="4" t="s">
         <v>115</v>
+      </c>
+      <c r="I227" s="1" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>